<commit_message>
Changes in the dashboard
</commit_message>
<xml_diff>
--- a/pj600-sla-dashboard/App_Data/Excel.xlsx
+++ b/pj600-sla-dashboard/App_Data/Excel.xlsx
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +442,20 @@
       </c>
       <c r="D5">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Dashboard and altered the file upload to upload a csv file and read and insert the content to the DB
</commit_message>
<xml_diff>
--- a/pj600-sla-dashboard/App_Data/Excel.xlsx
+++ b/pj600-sla-dashboard/App_Data/Excel.xlsx
@@ -369,7 +369,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,13 +446,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>

</xml_diff>